<commit_message>
Agent step completed: Incorporar análisis estadísticos avanzados (regresiones, correlaciones)
</commit_message>
<xml_diff>
--- a/datos_poblacion_abengibre.xlsx
+++ b/datos_poblacion_abengibre.xlsx
@@ -466,10 +466,8 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
+      <c r="C2" t="n">
+        <v>2023</v>
       </c>
       <c r="D2" t="n">
         <v>760</v>
@@ -486,10 +484,8 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
+      <c r="C3" t="n">
+        <v>2022</v>
       </c>
       <c r="D3" t="n">
         <v>739</v>
@@ -506,10 +502,8 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
+      <c r="C4" t="n">
+        <v>2021</v>
       </c>
       <c r="D4" t="n">
         <v>748</v>
@@ -526,10 +520,8 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
+      <c r="C5" t="n">
+        <v>2020</v>
       </c>
       <c r="D5" t="n">
         <v>761</v>
@@ -546,10 +538,8 @@
           <t>HOMBRE</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
+      <c r="C6" t="n">
+        <v>2023</v>
       </c>
       <c r="D6" t="n">
         <v>369</v>
@@ -566,10 +556,8 @@
           <t>HOMBRE</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
+      <c r="C7" t="n">
+        <v>2022</v>
       </c>
       <c r="D7" t="n">
         <v>363</v>
@@ -586,10 +574,8 @@
           <t>HOMBRE</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
+      <c r="C8" t="n">
+        <v>2021</v>
       </c>
       <c r="D8" t="n">
         <v>365</v>
@@ -606,10 +592,8 @@
           <t>HOMBRE</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
+      <c r="C9" t="n">
+        <v>2020</v>
       </c>
       <c r="D9" t="n">
         <v>365</v>
@@ -626,10 +610,8 @@
           <t>MUJER</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
+      <c r="C10" t="n">
+        <v>2023</v>
       </c>
       <c r="D10" t="n">
         <v>391</v>
@@ -646,10 +628,8 @@
           <t>MUJER</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
+      <c r="C11" t="n">
+        <v>2022</v>
       </c>
       <c r="D11" t="n">
         <v>376</v>
@@ -666,10 +646,8 @@
           <t>MUJER</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
+      <c r="C12" t="n">
+        <v>2021</v>
       </c>
       <c r="D12" t="n">
         <v>383</v>
@@ -686,10 +664,8 @@
           <t>MUJER</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
+      <c r="C13" t="n">
+        <v>2020</v>
       </c>
       <c r="D13" t="n">
         <v>396</v>

</xml_diff>